<commit_message>
Stoppage Report User Interface
Stoppage Report Generation User Interface Created and integrated to
server API successfully.
</commit_message>
<xml_diff>
--- a/Eclipse Settings/WheelSystem/FaultReport/report_305941.xlsx
+++ b/Eclipse Settings/WheelSystem/FaultReport/report_305941.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Flange Height Stops</t>
   </si>
@@ -53,16 +53,13 @@
     <t>Report End Date</t>
   </si>
   <si>
-    <t>1 (20%)</t>
-  </si>
-  <si>
     <t>0 (0%)</t>
   </si>
   <si>
-    <t>2017-01-01</t>
-  </si>
-  <si>
-    <t>2017-12-01</t>
+    <t>1 (100%)</t>
+  </si>
+  <si>
+    <t>2017-04-07</t>
   </si>
 </sst>
 </file>
@@ -464,25 +461,25 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>